<commit_message>
Bug fix. Add test.
Fix bug with get datetime value. Add test for this.
</commit_message>
<xml_diff>
--- a/UnitTest.OpenXml.Excel.Data/test.xlsx
+++ b/UnitTest.OpenXml.Excel.Data/test.xlsx
@@ -427,7 +427,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -470,7 +470,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1">
-        <v>36526</v>
+        <v>30402.288194444445</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>

</xml_diff>